<commit_message>
Added a script nr 2 that summarizes the data of each organoid and makes a QC tab with control data
</commit_message>
<xml_diff>
--- a/resources/FullscreenV2.xlsx
+++ b/resources/FullscreenV2.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhuismans/surfdrive/Promotie/12. STRATEGIC/Analyse 2.0/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A365A937-BB1F-BF4C-AD88-408B1C44F6E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF768D7D-0678-F84D-83FD-338AD06B2E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36360" yWindow="2920" windowWidth="36060" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$X$385</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1651,14 +1654,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:X385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:X1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M354" sqref="M354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="9" max="9" width="26.5" customWidth="1"/>
     <col min="21" max="21" width="25.33203125" customWidth="1"/>
     <col min="22" max="22" width="27.33203125" customWidth="1"/>
   </cols>
@@ -1737,7 +1742,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1769,7 +1774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>21</v>
       </c>
@@ -1798,7 +1803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>21</v>
       </c>
@@ -1827,7 +1832,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>21</v>
       </c>
@@ -1862,7 +1867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>21</v>
       </c>
@@ -1897,7 +1902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>21</v>
       </c>
@@ -1932,7 +1937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>21</v>
       </c>
@@ -1964,7 +1969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>21</v>
       </c>
@@ -1996,7 +2001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -2028,7 +2033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>21</v>
       </c>
@@ -2063,7 +2068,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>21</v>
       </c>
@@ -2098,7 +2103,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>21</v>
       </c>
@@ -2133,7 +2138,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>21</v>
       </c>
@@ -2168,7 +2173,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>21</v>
       </c>
@@ -2203,7 +2208,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>21</v>
       </c>
@@ -2238,7 +2243,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>21</v>
       </c>
@@ -2273,7 +2278,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>21</v>
       </c>
@@ -2308,7 +2313,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>21</v>
       </c>
@@ -2343,7 +2348,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>21</v>
       </c>
@@ -2378,7 +2383,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>21</v>
       </c>
@@ -2413,7 +2418,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>21</v>
       </c>
@@ -2448,7 +2453,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>21</v>
       </c>
@@ -2483,7 +2488,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>21</v>
       </c>
@@ -2518,7 +2523,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>21</v>
       </c>
@@ -2553,7 +2558,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>21</v>
       </c>
@@ -2573,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>21</v>
       </c>
@@ -2602,7 +2607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>21</v>
       </c>
@@ -2631,7 +2636,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>21</v>
       </c>
@@ -2666,7 +2671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>21</v>
       </c>
@@ -2701,7 +2706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>21</v>
       </c>
@@ -2736,7 +2741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>21</v>
       </c>
@@ -2771,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>21</v>
       </c>
@@ -2806,7 +2811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>21</v>
       </c>
@@ -2841,7 +2846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>21</v>
       </c>
@@ -2876,7 +2881,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="36" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>21</v>
       </c>
@@ -2911,7 +2916,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="37" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>21</v>
       </c>
@@ -2946,7 +2951,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="38" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>21</v>
       </c>
@@ -2981,7 +2986,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="39" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>21</v>
       </c>
@@ -3016,7 +3021,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="40" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>21</v>
       </c>
@@ -3051,7 +3056,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="41" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>21</v>
       </c>
@@ -3086,7 +3091,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="42" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>21</v>
       </c>
@@ -3121,7 +3126,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="43" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>21</v>
       </c>
@@ -3156,7 +3161,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="44" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>21</v>
       </c>
@@ -3191,7 +3196,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="45" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>21</v>
       </c>
@@ -3226,7 +3231,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="46" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>21</v>
       </c>
@@ -3261,7 +3266,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="47" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>21</v>
       </c>
@@ -3296,7 +3301,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="48" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>21</v>
       </c>
@@ -3331,7 +3336,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="49" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>21</v>
       </c>
@@ -3366,7 +3371,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="50" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>21</v>
       </c>
@@ -3386,7 +3391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>21</v>
       </c>
@@ -3415,7 +3420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>21</v>
       </c>
@@ -3444,7 +3449,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="53" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>21</v>
       </c>
@@ -3479,7 +3484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>21</v>
       </c>
@@ -3514,7 +3519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>21</v>
       </c>
@@ -3549,7 +3554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>21</v>
       </c>
@@ -3584,7 +3589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>21</v>
       </c>
@@ -3619,7 +3624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>21</v>
       </c>
@@ -3654,7 +3659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>21</v>
       </c>
@@ -3689,7 +3694,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="60" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>21</v>
       </c>
@@ -3724,7 +3729,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="61" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>21</v>
       </c>
@@ -3759,7 +3764,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="62" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>21</v>
       </c>
@@ -3794,7 +3799,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="63" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>21</v>
       </c>
@@ -3829,7 +3834,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="64" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>21</v>
       </c>
@@ -3864,7 +3869,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="65" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>21</v>
       </c>
@@ -3899,7 +3904,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="66" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>21</v>
       </c>
@@ -3934,7 +3939,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="67" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>21</v>
       </c>
@@ -3969,7 +3974,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="68" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>21</v>
       </c>
@@ -4004,7 +4009,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="69" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>21</v>
       </c>
@@ -4039,7 +4044,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="70" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>21</v>
       </c>
@@ -4074,7 +4079,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="71" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>21</v>
       </c>
@@ -4109,7 +4114,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="72" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>21</v>
       </c>
@@ -4144,7 +4149,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="73" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>21</v>
       </c>
@@ -4179,7 +4184,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="74" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>21</v>
       </c>
@@ -4199,7 +4204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>21</v>
       </c>
@@ -4228,7 +4233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>21</v>
       </c>
@@ -4257,7 +4262,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="77" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
         <v>21</v>
       </c>
@@ -4292,7 +4297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>21</v>
       </c>
@@ -4327,7 +4332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>21</v>
       </c>
@@ -4362,7 +4367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>21</v>
       </c>
@@ -4397,7 +4402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>21</v>
       </c>
@@ -4432,7 +4437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>21</v>
       </c>
@@ -4467,7 +4472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>21</v>
       </c>
@@ -4502,7 +4507,7 @@
         <v>1.0001485001485001E-2</v>
       </c>
     </row>
-    <row r="84" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>21</v>
       </c>
@@ -4537,7 +4542,7 @@
         <v>1.0001485001485001E-2</v>
       </c>
     </row>
-    <row r="85" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>21</v>
       </c>
@@ -4572,7 +4577,7 @@
         <v>1.0001485001485001E-2</v>
       </c>
     </row>
-    <row r="86" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>21</v>
       </c>
@@ -4607,7 +4612,7 @@
         <v>9.9970299970299995E-3</v>
       </c>
     </row>
-    <row r="87" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>21</v>
       </c>
@@ -4642,7 +4647,7 @@
         <v>9.9970299970299995E-3</v>
       </c>
     </row>
-    <row r="88" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>21</v>
       </c>
@@ -4677,7 +4682,7 @@
         <v>9.9970299970299995E-3</v>
       </c>
     </row>
-    <row r="89" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>21</v>
       </c>
@@ -4712,7 +4717,7 @@
         <v>9.9970299970299995E-3</v>
       </c>
     </row>
-    <row r="90" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
         <v>21</v>
       </c>
@@ -4747,7 +4752,7 @@
         <v>9.9970299970299995E-3</v>
       </c>
     </row>
-    <row r="91" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>21</v>
       </c>
@@ -4782,7 +4787,7 @@
         <v>9.9970299970299995E-3</v>
       </c>
     </row>
-    <row r="92" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>21</v>
       </c>
@@ -4817,7 +4822,7 @@
         <v>9.9970299970299995E-3</v>
       </c>
     </row>
-    <row r="93" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>21</v>
       </c>
@@ -4852,7 +4857,7 @@
         <v>9.9970299970299995E-3</v>
       </c>
     </row>
-    <row r="94" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>21</v>
       </c>
@@ -4887,7 +4892,7 @@
         <v>9.9970299970299995E-3</v>
       </c>
     </row>
-    <row r="95" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>21</v>
       </c>
@@ -4922,7 +4927,7 @@
         <v>9.9970299970299995E-3</v>
       </c>
     </row>
-    <row r="96" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
         <v>21</v>
       </c>
@@ -4957,7 +4962,7 @@
         <v>9.9970299970299995E-3</v>
       </c>
     </row>
-    <row r="97" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
         <v>21</v>
       </c>
@@ -4992,7 +4997,7 @@
         <v>9.9970299970299995E-3</v>
       </c>
     </row>
-    <row r="98" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>21</v>
       </c>
@@ -5012,7 +5017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>21</v>
       </c>
@@ -5041,7 +5046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>21</v>
       </c>
@@ -5070,7 +5075,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="101" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
         <v>21</v>
       </c>
@@ -5105,7 +5110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>21</v>
       </c>
@@ -5140,7 +5145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>21</v>
       </c>
@@ -5175,7 +5180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>21</v>
       </c>
@@ -5210,7 +5215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
         <v>21</v>
       </c>
@@ -5245,7 +5250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>21</v>
       </c>
@@ -5280,7 +5285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
         <v>21</v>
       </c>
@@ -5315,7 +5320,7 @@
         <v>9.9995049995050007E-3</v>
       </c>
     </row>
-    <row r="108" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
         <v>21</v>
       </c>
@@ -5350,7 +5355,7 @@
         <v>9.9995049995050007E-3</v>
       </c>
     </row>
-    <row r="109" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>21</v>
       </c>
@@ -5385,7 +5390,7 @@
         <v>9.9995049995050007E-3</v>
       </c>
     </row>
-    <row r="110" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
         <v>21</v>
       </c>
@@ -5420,7 +5425,7 @@
         <v>9.996534996535E-3</v>
       </c>
     </row>
-    <row r="111" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
         <v>21</v>
       </c>
@@ -5455,7 +5460,7 @@
         <v>9.996534996535E-3</v>
       </c>
     </row>
-    <row r="112" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
         <v>21</v>
       </c>
@@ -5490,7 +5495,7 @@
         <v>9.996534996535E-3</v>
       </c>
     </row>
-    <row r="113" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
         <v>21</v>
       </c>
@@ -5525,7 +5530,7 @@
         <v>9.996534996535E-3</v>
       </c>
     </row>
-    <row r="114" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>21</v>
       </c>
@@ -5560,7 +5565,7 @@
         <v>9.996534996535E-3</v>
       </c>
     </row>
-    <row r="115" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
         <v>21</v>
       </c>
@@ -5595,7 +5600,7 @@
         <v>9.996534996535E-3</v>
       </c>
     </row>
-    <row r="116" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
         <v>21</v>
       </c>
@@ -5630,7 +5635,7 @@
         <v>9.996534996535E-3</v>
       </c>
     </row>
-    <row r="117" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
         <v>21</v>
       </c>
@@ -5665,7 +5670,7 @@
         <v>9.996534996535E-3</v>
       </c>
     </row>
-    <row r="118" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
         <v>21</v>
       </c>
@@ -5700,7 +5705,7 @@
         <v>9.996534996535E-3</v>
       </c>
     </row>
-    <row r="119" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>21</v>
       </c>
@@ -5735,7 +5740,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="120" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
         <v>21</v>
       </c>
@@ -5770,7 +5775,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="121" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
         <v>21</v>
       </c>
@@ -5805,7 +5810,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="122" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
         <v>21</v>
       </c>
@@ -5825,7 +5830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
         <v>21</v>
       </c>
@@ -5854,7 +5859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
         <v>21</v>
       </c>
@@ -5883,7 +5888,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="125" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
         <v>21</v>
       </c>
@@ -5918,7 +5923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
         <v>21</v>
       </c>
@@ -5953,7 +5958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B127" t="s">
         <v>21</v>
       </c>
@@ -5988,7 +5993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
         <v>21</v>
       </c>
@@ -6023,7 +6028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>21</v>
       </c>
@@ -6058,7 +6063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
         <v>21</v>
       </c>
@@ -6093,7 +6098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>21</v>
       </c>
@@ -6128,7 +6133,7 @@
         <v>1.0002475002475E-2</v>
       </c>
     </row>
-    <row r="132" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
         <v>21</v>
       </c>
@@ -6163,7 +6168,7 @@
         <v>1.0002475002475E-2</v>
       </c>
     </row>
-    <row r="133" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
         <v>21</v>
       </c>
@@ -6198,7 +6203,7 @@
         <v>1.0002475002475E-2</v>
       </c>
     </row>
-    <row r="134" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
         <v>21</v>
       </c>
@@ -6233,7 +6238,7 @@
         <v>9.9945549945550001E-3</v>
       </c>
     </row>
-    <row r="135" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
         <v>21</v>
       </c>
@@ -6268,7 +6273,7 @@
         <v>9.9945549945550001E-3</v>
       </c>
     </row>
-    <row r="136" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
         <v>21</v>
       </c>
@@ -6303,7 +6308,7 @@
         <v>9.9945549945550001E-3</v>
       </c>
     </row>
-    <row r="137" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
         <v>21</v>
       </c>
@@ -6338,7 +6343,7 @@
         <v>9.9945549945550001E-3</v>
       </c>
     </row>
-    <row r="138" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
         <v>21</v>
       </c>
@@ -6373,7 +6378,7 @@
         <v>9.9945549945550001E-3</v>
       </c>
     </row>
-    <row r="139" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
         <v>21</v>
       </c>
@@ -6408,7 +6413,7 @@
         <v>9.9945549945550001E-3</v>
       </c>
     </row>
-    <row r="140" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
         <v>21</v>
       </c>
@@ -6443,7 +6448,7 @@
         <v>9.9945549945550001E-3</v>
       </c>
     </row>
-    <row r="141" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
         <v>21</v>
       </c>
@@ -6478,7 +6483,7 @@
         <v>9.9945549945550001E-3</v>
       </c>
     </row>
-    <row r="142" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
         <v>21</v>
       </c>
@@ -6513,7 +6518,7 @@
         <v>9.9945549945550001E-3</v>
       </c>
     </row>
-    <row r="143" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
         <v>21</v>
       </c>
@@ -6548,7 +6553,7 @@
         <v>9.996534996535E-3</v>
       </c>
     </row>
-    <row r="144" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
         <v>21</v>
       </c>
@@ -6583,7 +6588,7 @@
         <v>9.996534996535E-3</v>
       </c>
     </row>
-    <row r="145" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B145" t="s">
         <v>21</v>
       </c>
@@ -6618,7 +6623,7 @@
         <v>9.996534996535E-3</v>
       </c>
     </row>
-    <row r="146" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B146" t="s">
         <v>21</v>
       </c>
@@ -6638,7 +6643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
         <v>21</v>
       </c>
@@ -6667,7 +6672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B148" t="s">
         <v>21</v>
       </c>
@@ -6696,7 +6701,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="149" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B149" t="s">
         <v>21</v>
       </c>
@@ -6731,7 +6736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B150" t="s">
         <v>21</v>
       </c>
@@ -6766,7 +6771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B151" t="s">
         <v>21</v>
       </c>
@@ -6801,7 +6806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B152" t="s">
         <v>21</v>
       </c>
@@ -6836,7 +6841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B153" t="s">
         <v>21</v>
       </c>
@@ -6871,7 +6876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B154" t="s">
         <v>21</v>
       </c>
@@ -6906,7 +6911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
         <v>21</v>
       </c>
@@ -6941,7 +6946,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="156" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B156" t="s">
         <v>21</v>
       </c>
@@ -6976,7 +6981,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="157" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B157" t="s">
         <v>21</v>
       </c>
@@ -7011,7 +7016,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="158" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
         <v>21</v>
       </c>
@@ -7046,7 +7051,7 @@
         <v>1.0000495000495E-2</v>
       </c>
     </row>
-    <row r="159" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B159" t="s">
         <v>21</v>
       </c>
@@ -7081,7 +7086,7 @@
         <v>1.0000495000495E-2</v>
       </c>
     </row>
-    <row r="160" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B160" t="s">
         <v>21</v>
       </c>
@@ -7116,7 +7121,7 @@
         <v>1.0000495000495E-2</v>
       </c>
     </row>
-    <row r="161" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
         <v>21</v>
       </c>
@@ -7151,7 +7156,7 @@
         <v>1.0000495000495E-2</v>
       </c>
     </row>
-    <row r="162" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
         <v>21</v>
       </c>
@@ -7186,7 +7191,7 @@
         <v>1.0000495000495E-2</v>
       </c>
     </row>
-    <row r="163" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B163" t="s">
         <v>21</v>
       </c>
@@ -7221,7 +7226,7 @@
         <v>1.0000495000495E-2</v>
       </c>
     </row>
-    <row r="164" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
         <v>21</v>
       </c>
@@ -7256,7 +7261,7 @@
         <v>1.0000495000495E-2</v>
       </c>
     </row>
-    <row r="165" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B165" t="s">
         <v>21</v>
       </c>
@@ -7291,7 +7296,7 @@
         <v>1.0000495000495E-2</v>
       </c>
     </row>
-    <row r="166" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B166" t="s">
         <v>21</v>
       </c>
@@ -7326,7 +7331,7 @@
         <v>1.0000495000495E-2</v>
       </c>
     </row>
-    <row r="167" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
         <v>21</v>
       </c>
@@ -7361,7 +7366,7 @@
         <v>1.000198000198E-2</v>
       </c>
     </row>
-    <row r="168" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B168" t="s">
         <v>21</v>
       </c>
@@ -7396,7 +7401,7 @@
         <v>1.000198000198E-2</v>
       </c>
     </row>
-    <row r="169" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B169" t="s">
         <v>21</v>
       </c>
@@ -7431,7 +7436,7 @@
         <v>1.000198000198E-2</v>
       </c>
     </row>
-    <row r="170" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B170" t="s">
         <v>21</v>
       </c>
@@ -7451,7 +7456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B171" t="s">
         <v>21</v>
       </c>
@@ -7480,7 +7485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B172" t="s">
         <v>21</v>
       </c>
@@ -7509,7 +7514,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="173" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B173" t="s">
         <v>21</v>
       </c>
@@ -7544,7 +7549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B174" t="s">
         <v>21</v>
       </c>
@@ -7579,7 +7584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B175" t="s">
         <v>21</v>
       </c>
@@ -7614,7 +7619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B176" t="s">
         <v>21</v>
       </c>
@@ -7649,7 +7654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B177" t="s">
         <v>21</v>
       </c>
@@ -7684,7 +7689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B178" t="s">
         <v>21</v>
       </c>
@@ -7719,7 +7724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B179" t="s">
         <v>21</v>
       </c>
@@ -7754,7 +7759,7 @@
         <v>9.9993317493317496E-3</v>
       </c>
     </row>
-    <row r="180" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B180" t="s">
         <v>21</v>
       </c>
@@ -7789,7 +7794,7 @@
         <v>9.9993317493317496E-3</v>
       </c>
     </row>
-    <row r="181" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B181" t="s">
         <v>21</v>
       </c>
@@ -7824,7 +7829,7 @@
         <v>9.9993317493317496E-3</v>
       </c>
     </row>
-    <row r="182" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B182" t="s">
         <v>21</v>
       </c>
@@ -7859,7 +7864,7 @@
         <v>9.9995049995050007E-3</v>
       </c>
     </row>
-    <row r="183" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B183" t="s">
         <v>21</v>
       </c>
@@ -7894,7 +7899,7 @@
         <v>9.9995049995050007E-3</v>
       </c>
     </row>
-    <row r="184" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B184" t="s">
         <v>21</v>
       </c>
@@ -7929,7 +7934,7 @@
         <v>9.9995049995050007E-3</v>
       </c>
     </row>
-    <row r="185" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B185" t="s">
         <v>21</v>
       </c>
@@ -7964,7 +7969,7 @@
         <v>9.9995049995050007E-3</v>
       </c>
     </row>
-    <row r="186" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B186" t="s">
         <v>21</v>
       </c>
@@ -7999,7 +8004,7 @@
         <v>9.9995049995050007E-3</v>
       </c>
     </row>
-    <row r="187" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B187" t="s">
         <v>21</v>
       </c>
@@ -8034,7 +8039,7 @@
         <v>9.9995049995050007E-3</v>
       </c>
     </row>
-    <row r="188" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B188" t="s">
         <v>21</v>
       </c>
@@ -8069,7 +8074,7 @@
         <v>9.9995049995050007E-3</v>
       </c>
     </row>
-    <row r="189" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B189" t="s">
         <v>21</v>
       </c>
@@ -8104,7 +8109,7 @@
         <v>9.9995049995050007E-3</v>
       </c>
     </row>
-    <row r="190" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B190" t="s">
         <v>21</v>
       </c>
@@ -8139,7 +8144,7 @@
         <v>9.9995049995050007E-3</v>
       </c>
     </row>
-    <row r="191" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B191" t="s">
         <v>21</v>
       </c>
@@ -8174,7 +8179,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="192" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B192" t="s">
         <v>21</v>
       </c>
@@ -8209,7 +8214,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="193" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B193" t="s">
         <v>21</v>
       </c>
@@ -8244,7 +8249,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="194" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B194" t="s">
         <v>21</v>
       </c>
@@ -8279,7 +8284,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="195" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B195" t="s">
         <v>21</v>
       </c>
@@ -8314,7 +8319,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="196" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B196" t="s">
         <v>21</v>
       </c>
@@ -8349,7 +8354,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="197" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B197" t="s">
         <v>21</v>
       </c>
@@ -8384,7 +8389,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="198" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B198" t="s">
         <v>21</v>
       </c>
@@ -8419,7 +8424,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="199" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B199" t="s">
         <v>21</v>
       </c>
@@ -8454,7 +8459,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="200" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B200" t="s">
         <v>21</v>
       </c>
@@ -8489,7 +8494,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="201" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B201" t="s">
         <v>21</v>
       </c>
@@ -8524,7 +8529,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="202" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B202" t="s">
         <v>21</v>
       </c>
@@ -8559,7 +8564,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="203" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B203" t="s">
         <v>21</v>
       </c>
@@ -8594,7 +8599,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="204" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B204" t="s">
         <v>21</v>
       </c>
@@ -8629,7 +8634,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="205" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B205" t="s">
         <v>21</v>
       </c>
@@ -8664,7 +8669,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="206" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B206" t="s">
         <v>21</v>
       </c>
@@ -8699,7 +8704,7 @@
         <v>9.9891000998910007E-3</v>
       </c>
     </row>
-    <row r="207" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B207" t="s">
         <v>21</v>
       </c>
@@ -8734,7 +8739,7 @@
         <v>9.9891000998910007E-3</v>
       </c>
     </row>
-    <row r="208" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B208" t="s">
         <v>21</v>
       </c>
@@ -8883,7 +8888,7 @@
         <v>9.9940599940599902E-3</v>
       </c>
     </row>
-    <row r="212" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B212" t="s">
         <v>21</v>
       </c>
@@ -8918,7 +8923,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="213" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B213" t="s">
         <v>21</v>
       </c>
@@ -8953,7 +8958,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="214" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="214" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B214" t="s">
         <v>21</v>
       </c>
@@ -8988,7 +8993,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="215" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="215" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B215" t="s">
         <v>21</v>
       </c>
@@ -9023,7 +9028,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="216" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="216" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B216" t="s">
         <v>21</v>
       </c>
@@ -9058,7 +9063,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="217" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="217" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B217" t="s">
         <v>21</v>
       </c>
@@ -9093,7 +9098,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="218" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="218" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B218" t="s">
         <v>21</v>
       </c>
@@ -9128,7 +9133,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="219" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="219" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B219" t="s">
         <v>21</v>
       </c>
@@ -9163,7 +9168,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="220" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="220" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B220" t="s">
         <v>21</v>
       </c>
@@ -9198,7 +9203,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="221" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="221" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B221" t="s">
         <v>21</v>
       </c>
@@ -9233,7 +9238,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="222" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="222" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B222" t="s">
         <v>21</v>
       </c>
@@ -9268,7 +9273,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="223" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="223" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B223" t="s">
         <v>21</v>
       </c>
@@ -9303,7 +9308,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="224" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="224" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B224" t="s">
         <v>21</v>
       </c>
@@ -9338,7 +9343,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="225" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="225" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B225" t="s">
         <v>21</v>
       </c>
@@ -9373,7 +9378,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="226" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="226" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B226" t="s">
         <v>21</v>
       </c>
@@ -9408,7 +9413,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="227" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="227" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B227" t="s">
         <v>21</v>
       </c>
@@ -9443,7 +9448,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="228" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="228" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B228" t="s">
         <v>21</v>
       </c>
@@ -9478,7 +9483,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="229" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="229" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B229" t="s">
         <v>21</v>
       </c>
@@ -9513,7 +9518,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="230" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="230" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B230" t="s">
         <v>21</v>
       </c>
@@ -9548,7 +9553,7 @@
         <v>9.9891099891099792E-3</v>
       </c>
     </row>
-    <row r="231" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="231" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B231" t="s">
         <v>21</v>
       </c>
@@ -9583,7 +9588,7 @@
         <v>9.9891099891099792E-3</v>
       </c>
     </row>
-    <row r="232" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="232" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B232" t="s">
         <v>21</v>
       </c>
@@ -9732,7 +9737,7 @@
         <v>9.9940599940600006E-3</v>
       </c>
     </row>
-    <row r="236" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="236" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B236" t="s">
         <v>21</v>
       </c>
@@ -9767,7 +9772,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="237" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="237" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B237" t="s">
         <v>21</v>
       </c>
@@ -9802,7 +9807,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="238" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="238" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B238" t="s">
         <v>21</v>
       </c>
@@ -9837,7 +9842,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="239" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="239" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B239" t="s">
         <v>21</v>
       </c>
@@ -9872,7 +9877,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="240" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="240" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B240" t="s">
         <v>21</v>
       </c>
@@ -9907,7 +9912,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="241" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="241" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B241" t="s">
         <v>21</v>
       </c>
@@ -9942,7 +9947,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="242" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="242" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B242" t="s">
         <v>21</v>
       </c>
@@ -9977,7 +9982,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="243" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="243" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B243" t="s">
         <v>21</v>
       </c>
@@ -10012,7 +10017,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="244" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="244" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B244" t="s">
         <v>21</v>
       </c>
@@ -10047,7 +10052,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="245" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="245" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B245" t="s">
         <v>21</v>
       </c>
@@ -10082,7 +10087,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="246" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="246" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B246" t="s">
         <v>21</v>
       </c>
@@ -10117,7 +10122,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="247" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="247" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B247" t="s">
         <v>21</v>
       </c>
@@ -10152,7 +10157,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="248" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="248" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B248" t="s">
         <v>21</v>
       </c>
@@ -10187,7 +10192,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="249" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="249" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B249" t="s">
         <v>21</v>
       </c>
@@ -10222,7 +10227,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="250" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="250" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B250" t="s">
         <v>21</v>
       </c>
@@ -10257,7 +10262,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="251" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="251" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B251" t="s">
         <v>21</v>
       </c>
@@ -10292,7 +10297,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="252" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="252" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B252" t="s">
         <v>21</v>
       </c>
@@ -10327,7 +10332,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="253" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="253" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B253" t="s">
         <v>21</v>
       </c>
@@ -10362,7 +10367,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="254" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="254" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B254" t="s">
         <v>21</v>
       </c>
@@ -10397,7 +10402,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="255" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="255" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B255" t="s">
         <v>21</v>
       </c>
@@ -10432,7 +10437,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="256" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="256" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B256" t="s">
         <v>21</v>
       </c>
@@ -10581,7 +10586,7 @@
         <v>9.9940599940599902E-3</v>
       </c>
     </row>
-    <row r="260" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="260" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B260" t="s">
         <v>21</v>
       </c>
@@ -10616,7 +10621,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="261" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="261" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B261" t="s">
         <v>21</v>
       </c>
@@ -10651,7 +10656,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="262" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="262" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B262" t="s">
         <v>21</v>
       </c>
@@ -10686,7 +10691,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="263" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="263" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B263" t="s">
         <v>21</v>
       </c>
@@ -10721,7 +10726,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="264" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="264" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B264" t="s">
         <v>21</v>
       </c>
@@ -10756,7 +10761,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="265" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="265" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B265" t="s">
         <v>21</v>
       </c>
@@ -10791,7 +10796,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="266" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="266" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B266" t="s">
         <v>21</v>
       </c>
@@ -10826,7 +10831,7 @@
         <v>9.9950499950499996E-3</v>
       </c>
     </row>
-    <row r="267" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="267" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B267" t="s">
         <v>21</v>
       </c>
@@ -10861,7 +10866,7 @@
         <v>9.9950499950499996E-3</v>
       </c>
     </row>
-    <row r="268" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="268" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B268" t="s">
         <v>21</v>
       </c>
@@ -10896,7 +10901,7 @@
         <v>9.9950499950499996E-3</v>
       </c>
     </row>
-    <row r="269" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="269" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B269" t="s">
         <v>21</v>
       </c>
@@ -10931,7 +10936,7 @@
         <v>9.9950499950499996E-3</v>
       </c>
     </row>
-    <row r="270" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="270" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B270" t="s">
         <v>21</v>
       </c>
@@ -10966,7 +10971,7 @@
         <v>9.9950499950499996E-3</v>
       </c>
     </row>
-    <row r="271" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="271" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B271" t="s">
         <v>21</v>
       </c>
@@ -11001,7 +11006,7 @@
         <v>9.9950499950499996E-3</v>
       </c>
     </row>
-    <row r="272" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="272" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B272" t="s">
         <v>21</v>
       </c>
@@ -11036,7 +11041,7 @@
         <v>9.9950499950499996E-3</v>
       </c>
     </row>
-    <row r="273" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="273" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B273" t="s">
         <v>21</v>
       </c>
@@ -11071,7 +11076,7 @@
         <v>9.9950499950499996E-3</v>
       </c>
     </row>
-    <row r="274" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="274" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B274" t="s">
         <v>21</v>
       </c>
@@ -11106,7 +11111,7 @@
         <v>9.9950499950499996E-3</v>
       </c>
     </row>
-    <row r="275" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="275" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B275" t="s">
         <v>21</v>
       </c>
@@ -11141,7 +11146,7 @@
         <v>1.0000495000495E-2</v>
       </c>
     </row>
-    <row r="276" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="276" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B276" t="s">
         <v>21</v>
       </c>
@@ -11176,7 +11181,7 @@
         <v>1.0000495000495E-2</v>
       </c>
     </row>
-    <row r="277" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="277" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B277" t="s">
         <v>21</v>
       </c>
@@ -11211,7 +11216,7 @@
         <v>1.0000495000495E-2</v>
       </c>
     </row>
-    <row r="278" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="278" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B278" t="s">
         <v>21</v>
       </c>
@@ -11246,7 +11251,7 @@
         <v>9.9970299970299995E-3</v>
       </c>
     </row>
-    <row r="279" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="279" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B279" t="s">
         <v>21</v>
       </c>
@@ -11281,7 +11286,7 @@
         <v>9.9970299970299995E-3</v>
       </c>
     </row>
-    <row r="280" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="280" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B280" t="s">
         <v>21</v>
       </c>
@@ -11430,7 +11435,7 @@
         <v>1.000198000198E-2</v>
       </c>
     </row>
-    <row r="284" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="284" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B284" t="s">
         <v>21</v>
       </c>
@@ -11465,7 +11470,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="285" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="285" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B285" t="s">
         <v>21</v>
       </c>
@@ -11500,7 +11505,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="286" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="286" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B286" t="s">
         <v>21</v>
       </c>
@@ -11535,7 +11540,7 @@
         <v>9.9990099990099994E-3</v>
       </c>
     </row>
-    <row r="287" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="287" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B287" t="s">
         <v>21</v>
       </c>
@@ -11570,7 +11575,7 @@
         <v>9.9980199980200003E-3</v>
       </c>
     </row>
-    <row r="288" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="288" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B288" t="s">
         <v>21</v>
       </c>
@@ -11605,7 +11610,7 @@
         <v>9.9980199980200003E-3</v>
       </c>
     </row>
-    <row r="289" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="289" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B289" t="s">
         <v>21</v>
       </c>
@@ -11640,7 +11645,7 @@
         <v>9.9980199980200003E-3</v>
       </c>
     </row>
-    <row r="290" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="290" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B290" t="s">
         <v>21</v>
       </c>
@@ -11675,7 +11680,7 @@
         <v>9.9940599940599902E-3</v>
       </c>
     </row>
-    <row r="291" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="291" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B291" t="s">
         <v>21</v>
       </c>
@@ -11710,7 +11715,7 @@
         <v>9.9940599940599902E-3</v>
       </c>
     </row>
-    <row r="292" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="292" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B292" t="s">
         <v>21</v>
       </c>
@@ -11745,7 +11750,7 @@
         <v>9.9940599940599902E-3</v>
       </c>
     </row>
-    <row r="293" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="293" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B293" t="s">
         <v>21</v>
       </c>
@@ -11780,7 +11785,7 @@
         <v>9.9940599940599902E-3</v>
       </c>
     </row>
-    <row r="294" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="294" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B294" t="s">
         <v>21</v>
       </c>
@@ -11815,7 +11820,7 @@
         <v>9.9940599940599902E-3</v>
       </c>
     </row>
-    <row r="295" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="295" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B295" t="s">
         <v>21</v>
       </c>
@@ -11850,7 +11855,7 @@
         <v>9.9940599940599902E-3</v>
       </c>
     </row>
-    <row r="296" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="296" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B296" t="s">
         <v>21</v>
       </c>
@@ -11885,7 +11890,7 @@
         <v>9.9940599940599902E-3</v>
       </c>
     </row>
-    <row r="297" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="297" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B297" t="s">
         <v>21</v>
       </c>
@@ -11920,7 +11925,7 @@
         <v>9.9940599940599902E-3</v>
       </c>
     </row>
-    <row r="298" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="298" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B298" t="s">
         <v>21</v>
       </c>
@@ -11955,7 +11960,7 @@
         <v>9.9940599940599902E-3</v>
       </c>
     </row>
-    <row r="299" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="299" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B299" t="s">
         <v>21</v>
       </c>
@@ -11990,7 +11995,7 @@
         <v>1.0002475002475E-2</v>
       </c>
     </row>
-    <row r="300" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="300" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B300" t="s">
         <v>21</v>
       </c>
@@ -12025,7 +12030,7 @@
         <v>1.0002475002475E-2</v>
       </c>
     </row>
-    <row r="301" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="301" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B301" t="s">
         <v>21</v>
       </c>
@@ -12060,7 +12065,7 @@
         <v>1.0002475002475E-2</v>
       </c>
     </row>
-    <row r="302" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="302" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B302" t="s">
         <v>21</v>
       </c>
@@ -12095,7 +12100,7 @@
         <v>1.0002970002969999E-2</v>
       </c>
     </row>
-    <row r="303" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="303" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B303" t="s">
         <v>21</v>
       </c>
@@ -12130,7 +12135,7 @@
         <v>1.0002970002969999E-2</v>
       </c>
     </row>
-    <row r="304" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="304" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B304" t="s">
         <v>21</v>
       </c>
@@ -12279,7 +12284,7 @@
         <v>9.9950499950499996E-3</v>
       </c>
     </row>
-    <row r="308" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="308" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B308" t="s">
         <v>21</v>
       </c>
@@ -12314,7 +12319,7 @@
         <v>1.000198000198E-2</v>
       </c>
     </row>
-    <row r="309" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="309" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B309" t="s">
         <v>21</v>
       </c>
@@ -12330,6 +12335,9 @@
       <c r="I309" t="s">
         <v>249</v>
       </c>
+      <c r="J309">
+        <v>0.32670032670030003</v>
+      </c>
       <c r="K309">
         <v>0.32670032670030003</v>
       </c>
@@ -12346,7 +12354,7 @@
         <v>1.000198000198E-2</v>
       </c>
     </row>
-    <row r="310" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="310" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B310" t="s">
         <v>21</v>
       </c>
@@ -12362,6 +12370,9 @@
       <c r="I310" t="s">
         <v>249</v>
       </c>
+      <c r="J310">
+        <v>0.32670032670030003</v>
+      </c>
       <c r="K310">
         <v>0.32670032670030003</v>
       </c>
@@ -12378,7 +12389,7 @@
         <v>1.000198000198E-2</v>
       </c>
     </row>
-    <row r="311" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="311" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B311" t="s">
         <v>21</v>
       </c>
@@ -12394,6 +12405,9 @@
       <c r="I311" t="s">
         <v>253</v>
       </c>
+      <c r="J311">
+        <v>1.287001287001E-2</v>
+      </c>
       <c r="K311">
         <v>1.287001287001E-2</v>
       </c>
@@ -12410,7 +12424,7 @@
         <v>1.000198000198E-2</v>
       </c>
     </row>
-    <row r="312" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="312" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B312" t="s">
         <v>21</v>
       </c>
@@ -12426,6 +12440,9 @@
       <c r="I312" t="s">
         <v>253</v>
       </c>
+      <c r="J312">
+        <v>1.287001287001E-2</v>
+      </c>
       <c r="K312">
         <v>1.287001287001E-2</v>
       </c>
@@ -12442,7 +12459,7 @@
         <v>1.000198000198E-2</v>
       </c>
     </row>
-    <row r="313" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="313" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B313" t="s">
         <v>21</v>
       </c>
@@ -12458,6 +12475,9 @@
       <c r="I313" t="s">
         <v>253</v>
       </c>
+      <c r="J313">
+        <v>1.287001287001E-2</v>
+      </c>
       <c r="K313">
         <v>1.287001287001E-2</v>
       </c>
@@ -12474,7 +12494,7 @@
         <v>1.000198000198E-2</v>
       </c>
     </row>
-    <row r="314" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="314" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B314" t="s">
         <v>21</v>
       </c>
@@ -12490,6 +12510,9 @@
       <c r="I314" t="s">
         <v>225</v>
       </c>
+      <c r="J314">
+        <v>5.4450054450050002E-2</v>
+      </c>
       <c r="O314">
         <v>5.4450054450050002E-2</v>
       </c>
@@ -12506,7 +12529,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="315" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="315" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B315" t="s">
         <v>21</v>
       </c>
@@ -12522,6 +12545,9 @@
       <c r="I315" t="s">
         <v>225</v>
       </c>
+      <c r="J315">
+        <v>5.4450054450050002E-2</v>
+      </c>
       <c r="O315">
         <v>5.4450054450050002E-2</v>
       </c>
@@ -12538,7 +12564,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="316" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="316" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B316" t="s">
         <v>21</v>
       </c>
@@ -12554,6 +12580,9 @@
       <c r="I316" t="s">
         <v>225</v>
       </c>
+      <c r="J316">
+        <v>5.4450054450050002E-2</v>
+      </c>
       <c r="O316">
         <v>5.4450054450050002E-2</v>
       </c>
@@ -12570,7 +12599,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="317" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="317" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B317" t="s">
         <v>21</v>
       </c>
@@ -12586,6 +12615,9 @@
       <c r="I317" t="s">
         <v>229</v>
       </c>
+      <c r="J317">
+        <v>5.4450054450050002E-2</v>
+      </c>
       <c r="O317">
         <v>5.4450054450050002E-2</v>
       </c>
@@ -12602,7 +12634,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="318" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="318" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B318" t="s">
         <v>21</v>
       </c>
@@ -12618,6 +12650,9 @@
       <c r="I318" t="s">
         <v>229</v>
       </c>
+      <c r="J318">
+        <v>5.4450054450050002E-2</v>
+      </c>
       <c r="O318">
         <v>5.4450054450050002E-2</v>
       </c>
@@ -12634,7 +12669,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="319" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="319" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B319" t="s">
         <v>21</v>
       </c>
@@ -12650,6 +12685,9 @@
       <c r="I319" t="s">
         <v>229</v>
       </c>
+      <c r="J319">
+        <v>5.4450054450050002E-2</v>
+      </c>
       <c r="O319">
         <v>5.4450054450050002E-2</v>
       </c>
@@ -12666,7 +12704,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="320" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="320" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B320" t="s">
         <v>21</v>
       </c>
@@ -12682,6 +12720,9 @@
       <c r="I320" t="s">
         <v>233</v>
       </c>
+      <c r="J320">
+        <v>5.4450054450050002E-2</v>
+      </c>
       <c r="P320">
         <v>5.4450054450050002E-2</v>
       </c>
@@ -12698,7 +12739,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="321" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="321" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B321" t="s">
         <v>21</v>
       </c>
@@ -12714,6 +12755,9 @@
       <c r="I321" t="s">
         <v>233</v>
       </c>
+      <c r="J321">
+        <v>5.4450054450050002E-2</v>
+      </c>
       <c r="P321">
         <v>5.4450054450050002E-2</v>
       </c>
@@ -12730,7 +12774,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="322" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="322" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B322" t="s">
         <v>21</v>
       </c>
@@ -12746,6 +12790,9 @@
       <c r="I322" t="s">
         <v>233</v>
       </c>
+      <c r="J322">
+        <v>5.4450054450050002E-2</v>
+      </c>
       <c r="P322">
         <v>5.4450054450050002E-2</v>
       </c>
@@ -12762,7 +12809,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="323" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="323" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B323" t="s">
         <v>21</v>
       </c>
@@ -12778,6 +12825,9 @@
       <c r="I323" t="s">
         <v>237</v>
       </c>
+      <c r="J323">
+        <v>4.455004455004E-3</v>
+      </c>
       <c r="N323">
         <v>6.9300069300070001E-3</v>
       </c>
@@ -12794,7 +12844,7 @@
         <v>9.9970299970299995E-3</v>
       </c>
     </row>
-    <row r="324" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="324" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B324" t="s">
         <v>21</v>
       </c>
@@ -12810,6 +12860,9 @@
       <c r="I324" t="s">
         <v>237</v>
       </c>
+      <c r="J324">
+        <v>4.455004455004E-3</v>
+      </c>
       <c r="N324">
         <v>6.9300069300070001E-3</v>
       </c>
@@ -12826,7 +12879,7 @@
         <v>9.9970299970299995E-3</v>
       </c>
     </row>
-    <row r="325" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="325" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B325" t="s">
         <v>21</v>
       </c>
@@ -12842,6 +12895,9 @@
       <c r="I325" t="s">
         <v>237</v>
       </c>
+      <c r="J325">
+        <v>4.455004455004E-3</v>
+      </c>
       <c r="N325">
         <v>6.9300069300070001E-3</v>
       </c>
@@ -12858,7 +12914,7 @@
         <v>9.9970299970299995E-3</v>
       </c>
     </row>
-    <row r="326" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="326" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B326" t="s">
         <v>21</v>
       </c>
@@ -12874,6 +12930,9 @@
       <c r="I326" t="s">
         <v>241</v>
       </c>
+      <c r="J326">
+        <v>3.7125037125040001E-3</v>
+      </c>
       <c r="S326">
         <v>7.9200079200080001E-2</v>
       </c>
@@ -12890,7 +12949,7 @@
         <v>9.9945549945549897E-3</v>
       </c>
     </row>
-    <row r="327" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="327" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B327" t="s">
         <v>21</v>
       </c>
@@ -12906,6 +12965,9 @@
       <c r="I327" t="s">
         <v>241</v>
       </c>
+      <c r="J327">
+        <v>3.7125037125040001E-3</v>
+      </c>
       <c r="S327">
         <v>7.9200079200080001E-2</v>
       </c>
@@ -12922,7 +12984,7 @@
         <v>9.9945549945549897E-3</v>
       </c>
     </row>
-    <row r="328" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="328" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B328" t="s">
         <v>21</v>
       </c>
@@ -12938,6 +13000,9 @@
       <c r="I328" t="s">
         <v>241</v>
       </c>
+      <c r="J328">
+        <v>3.7125037125040001E-3</v>
+      </c>
       <c r="S328">
         <v>7.9200079200080001E-2</v>
       </c>
@@ -12970,6 +13035,9 @@
       <c r="I329" t="s">
         <v>245</v>
       </c>
+      <c r="J329">
+        <v>3.7125037125040001E-3</v>
+      </c>
       <c r="O329">
         <v>0.17325017325020001</v>
       </c>
@@ -13005,6 +13073,9 @@
       <c r="I330" t="s">
         <v>245</v>
       </c>
+      <c r="J330">
+        <v>3.7125037125040001E-3</v>
+      </c>
       <c r="O330">
         <v>0.17325017325020001</v>
       </c>
@@ -13040,6 +13111,9 @@
       <c r="I331" t="s">
         <v>245</v>
       </c>
+      <c r="J331">
+        <v>3.7125037125040001E-3</v>
+      </c>
       <c r="O331">
         <v>0.17325017325020001</v>
       </c>
@@ -13059,7 +13133,7 @@
         <v>1.0001485001485001E-2</v>
       </c>
     </row>
-    <row r="332" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="332" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B332" t="s">
         <v>21</v>
       </c>
@@ -13075,6 +13149,9 @@
       <c r="I332" t="s">
         <v>249</v>
       </c>
+      <c r="J332">
+        <v>7.9200079200080001E-2</v>
+      </c>
       <c r="K332">
         <v>7.9200079200080001E-2</v>
       </c>
@@ -13091,7 +13168,7 @@
         <v>9.9970299970299995E-3</v>
       </c>
     </row>
-    <row r="333" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="333" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B333" t="s">
         <v>21</v>
       </c>
@@ -13107,6 +13184,9 @@
       <c r="I333" t="s">
         <v>249</v>
       </c>
+      <c r="J333">
+        <v>7.9200079200080001E-2</v>
+      </c>
       <c r="K333">
         <v>7.9200079200080001E-2</v>
       </c>
@@ -13123,7 +13203,7 @@
         <v>9.9970299970299995E-3</v>
       </c>
     </row>
-    <row r="334" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="334" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B334" t="s">
         <v>21</v>
       </c>
@@ -13139,6 +13219,9 @@
       <c r="I334" t="s">
         <v>249</v>
       </c>
+      <c r="J334">
+        <v>7.9200079200080001E-2</v>
+      </c>
       <c r="K334">
         <v>7.9200079200080001E-2</v>
       </c>
@@ -13155,7 +13238,7 @@
         <v>9.9970299970299995E-3</v>
       </c>
     </row>
-    <row r="335" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="335" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B335" t="s">
         <v>21</v>
       </c>
@@ -13171,6 +13254,9 @@
       <c r="I335" t="s">
         <v>253</v>
       </c>
+      <c r="J335">
+        <v>4.455004455004E-3</v>
+      </c>
       <c r="K335">
         <v>4.455004455004E-3</v>
       </c>
@@ -13187,7 +13273,7 @@
         <v>1.0003465003465E-2</v>
       </c>
     </row>
-    <row r="336" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="336" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B336" t="s">
         <v>21</v>
       </c>
@@ -13203,6 +13289,9 @@
       <c r="I336" t="s">
         <v>253</v>
       </c>
+      <c r="J336">
+        <v>4.455004455004E-3</v>
+      </c>
       <c r="K336">
         <v>4.455004455004E-3</v>
       </c>
@@ -13219,7 +13308,7 @@
         <v>1.0003465003465E-2</v>
       </c>
     </row>
-    <row r="337" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="337" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B337" t="s">
         <v>21</v>
       </c>
@@ -13235,6 +13324,9 @@
       <c r="I337" t="s">
         <v>253</v>
       </c>
+      <c r="J337">
+        <v>4.455004455004E-3</v>
+      </c>
       <c r="K337">
         <v>4.455004455004E-3</v>
       </c>
@@ -13251,7 +13343,7 @@
         <v>1.0003465003465E-2</v>
       </c>
     </row>
-    <row r="338" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="338" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B338" t="s">
         <v>21</v>
       </c>
@@ -13267,6 +13359,9 @@
       <c r="I338" t="s">
         <v>225</v>
       </c>
+      <c r="J338">
+        <v>1.485001485001E-2</v>
+      </c>
       <c r="O338">
         <v>1.485001485001E-2</v>
       </c>
@@ -13283,7 +13378,7 @@
         <v>1.000198000198E-2</v>
       </c>
     </row>
-    <row r="339" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="339" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B339" t="s">
         <v>21</v>
       </c>
@@ -13299,6 +13394,9 @@
       <c r="I339" t="s">
         <v>225</v>
       </c>
+      <c r="J339">
+        <v>1.485001485001E-2</v>
+      </c>
       <c r="O339">
         <v>1.485001485001E-2</v>
       </c>
@@ -13315,7 +13413,7 @@
         <v>1.000198000198E-2</v>
       </c>
     </row>
-    <row r="340" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="340" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B340" t="s">
         <v>21</v>
       </c>
@@ -13331,6 +13429,9 @@
       <c r="I340" t="s">
         <v>225</v>
       </c>
+      <c r="J340">
+        <v>1.485001485001E-2</v>
+      </c>
       <c r="O340">
         <v>1.485001485001E-2</v>
       </c>
@@ -13347,7 +13448,7 @@
         <v>1.000198000198E-2</v>
       </c>
     </row>
-    <row r="341" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="341" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B341" t="s">
         <v>21</v>
       </c>
@@ -13363,6 +13464,9 @@
       <c r="I341" t="s">
         <v>229</v>
       </c>
+      <c r="J341">
+        <v>1.485001485001E-2</v>
+      </c>
       <c r="O341">
         <v>1.485001485001E-2</v>
       </c>
@@ -13379,7 +13483,7 @@
         <v>1.000198000198E-2</v>
       </c>
     </row>
-    <row r="342" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="342" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B342" t="s">
         <v>21</v>
       </c>
@@ -13395,6 +13499,9 @@
       <c r="I342" t="s">
         <v>229</v>
       </c>
+      <c r="J342">
+        <v>1.485001485001E-2</v>
+      </c>
       <c r="O342">
         <v>1.485001485001E-2</v>
       </c>
@@ -13411,7 +13518,7 @@
         <v>1.000198000198E-2</v>
       </c>
     </row>
-    <row r="343" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="343" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B343" t="s">
         <v>21</v>
       </c>
@@ -13427,6 +13534,9 @@
       <c r="I343" t="s">
         <v>229</v>
       </c>
+      <c r="J343">
+        <v>1.485001485001E-2</v>
+      </c>
       <c r="O343">
         <v>1.485001485001E-2</v>
       </c>
@@ -13443,7 +13553,7 @@
         <v>1.000198000198E-2</v>
       </c>
     </row>
-    <row r="344" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="344" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B344" t="s">
         <v>21</v>
       </c>
@@ -13459,6 +13569,9 @@
       <c r="I344" t="s">
         <v>233</v>
       </c>
+      <c r="J344">
+        <v>1.485001485001E-2</v>
+      </c>
       <c r="P344">
         <v>1.485001485001E-2</v>
       </c>
@@ -13475,7 +13588,7 @@
         <v>1.000198000198E-2</v>
       </c>
     </row>
-    <row r="345" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="345" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B345" t="s">
         <v>21</v>
       </c>
@@ -13491,6 +13604,9 @@
       <c r="I345" t="s">
         <v>233</v>
       </c>
+      <c r="J345">
+        <v>1.485001485001E-2</v>
+      </c>
       <c r="P345">
         <v>1.485001485001E-2</v>
       </c>
@@ -13507,7 +13623,7 @@
         <v>1.000198000198E-2</v>
       </c>
     </row>
-    <row r="346" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="346" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B346" t="s">
         <v>21</v>
       </c>
@@ -13523,6 +13639,9 @@
       <c r="I346" t="s">
         <v>233</v>
       </c>
+      <c r="J346">
+        <v>1.485001485001E-2</v>
+      </c>
       <c r="P346">
         <v>1.485001485001E-2</v>
       </c>
@@ -13539,7 +13658,7 @@
         <v>1.000198000198E-2</v>
       </c>
     </row>
-    <row r="347" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="347" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B347" t="s">
         <v>21</v>
       </c>
@@ -13555,6 +13674,9 @@
       <c r="I347" t="s">
         <v>237</v>
       </c>
+      <c r="J347">
+        <v>1.485001485001E-3</v>
+      </c>
       <c r="N347">
         <v>1.980001980002E-3</v>
       </c>
@@ -13571,7 +13693,7 @@
         <v>1.0001485001485001E-2</v>
       </c>
     </row>
-    <row r="348" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="348" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B348" t="s">
         <v>21</v>
       </c>
@@ -13587,6 +13709,9 @@
       <c r="I348" t="s">
         <v>237</v>
       </c>
+      <c r="J348">
+        <v>1.485001485001E-3</v>
+      </c>
       <c r="N348">
         <v>1.980001980002E-3</v>
       </c>
@@ -13603,7 +13728,7 @@
         <v>1.0001485001485001E-2</v>
       </c>
     </row>
-    <row r="349" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="349" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B349" t="s">
         <v>21</v>
       </c>
@@ -13619,6 +13744,9 @@
       <c r="I349" t="s">
         <v>237</v>
       </c>
+      <c r="J349">
+        <v>1.485001485001E-3</v>
+      </c>
       <c r="N349">
         <v>1.980001980002E-3</v>
       </c>
@@ -13635,7 +13763,7 @@
         <v>1.0001485001485001E-2</v>
       </c>
     </row>
-    <row r="350" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="350" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B350" t="s">
         <v>21</v>
       </c>
@@ -13651,6 +13779,9 @@
       <c r="I350" t="s">
         <v>241</v>
       </c>
+      <c r="J350">
+        <v>1.485001485001E-3</v>
+      </c>
       <c r="S350">
         <v>1.980001980002E-2</v>
       </c>
@@ -13667,7 +13798,7 @@
         <v>1.000396000396E-2</v>
       </c>
     </row>
-    <row r="351" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="351" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B351" t="s">
         <v>21</v>
       </c>
@@ -13683,6 +13814,9 @@
       <c r="I351" t="s">
         <v>241</v>
       </c>
+      <c r="J351">
+        <v>1.485001485001E-3</v>
+      </c>
       <c r="S351">
         <v>1.980001980002E-2</v>
       </c>
@@ -13699,7 +13833,7 @@
         <v>1.000396000396E-2</v>
       </c>
     </row>
-    <row r="352" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="352" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B352" t="s">
         <v>21</v>
       </c>
@@ -13715,6 +13849,9 @@
       <c r="I352" t="s">
         <v>241</v>
       </c>
+      <c r="J352">
+        <v>1.485001485001E-3</v>
+      </c>
       <c r="S352">
         <v>1.980001980002E-2</v>
       </c>
@@ -13747,6 +13884,9 @@
       <c r="I353" t="s">
         <v>245</v>
       </c>
+      <c r="J353">
+        <v>1.485001485001E-3</v>
+      </c>
       <c r="O353">
         <v>0.17325017325020001</v>
       </c>
@@ -13782,6 +13922,9 @@
       <c r="I354" t="s">
         <v>245</v>
       </c>
+      <c r="J354">
+        <v>1.485001485001E-3</v>
+      </c>
       <c r="O354">
         <v>0.17325017325020001</v>
       </c>
@@ -13817,6 +13960,9 @@
       <c r="I355" t="s">
         <v>245</v>
       </c>
+      <c r="J355">
+        <v>1.485001485001E-3</v>
+      </c>
       <c r="O355">
         <v>0.17325017325020001</v>
       </c>
@@ -13836,7 +13982,7 @@
         <v>9.9970299970299995E-3</v>
       </c>
     </row>
-    <row r="356" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="356" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B356" t="s">
         <v>21</v>
       </c>
@@ -13852,6 +13998,9 @@
       <c r="I356" t="s">
         <v>249</v>
       </c>
+      <c r="J356">
+        <v>1.980001980002E-2</v>
+      </c>
       <c r="K356">
         <v>1.980001980002E-2</v>
       </c>
@@ -13868,7 +14017,7 @@
         <v>1.0000990000989999E-2</v>
       </c>
     </row>
-    <row r="357" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="357" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B357" t="s">
         <v>21</v>
       </c>
@@ -13884,6 +14033,9 @@
       <c r="I357" t="s">
         <v>249</v>
       </c>
+      <c r="J357">
+        <v>1.980001980002E-2</v>
+      </c>
       <c r="K357">
         <v>1.980001980002E-2</v>
       </c>
@@ -13900,7 +14052,7 @@
         <v>1.0000990000989999E-2</v>
       </c>
     </row>
-    <row r="358" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="358" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B358" t="s">
         <v>21</v>
       </c>
@@ -13916,6 +14068,9 @@
       <c r="I358" t="s">
         <v>249</v>
       </c>
+      <c r="J358">
+        <v>1.980001980002E-2</v>
+      </c>
       <c r="K358">
         <v>1.980001980002E-2</v>
       </c>
@@ -13932,7 +14087,7 @@
         <v>1.0000990000989999E-2</v>
       </c>
     </row>
-    <row r="359" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="359" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B359" t="s">
         <v>21</v>
       </c>
@@ -13948,6 +14103,9 @@
       <c r="I359" t="s">
         <v>253</v>
       </c>
+      <c r="J359">
+        <v>1.485001485001E-3</v>
+      </c>
       <c r="K359">
         <v>1.485001485001E-3</v>
       </c>
@@ -13964,7 +14122,7 @@
         <v>1.0000495000495E-2</v>
       </c>
     </row>
-    <row r="360" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="360" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B360" t="s">
         <v>21</v>
       </c>
@@ -13980,6 +14138,9 @@
       <c r="I360" t="s">
         <v>253</v>
       </c>
+      <c r="J360">
+        <v>1.485001485001E-3</v>
+      </c>
       <c r="K360">
         <v>1.485001485001E-3</v>
       </c>
@@ -13996,7 +14157,7 @@
         <v>1.0000495000495E-2</v>
       </c>
     </row>
-    <row r="361" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="361" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B361" t="s">
         <v>21</v>
       </c>
@@ -14012,6 +14173,9 @@
       <c r="I361" t="s">
         <v>253</v>
       </c>
+      <c r="J361">
+        <v>1.485001485001E-3</v>
+      </c>
       <c r="K361">
         <v>1.485001485001E-3</v>
       </c>
@@ -14028,7 +14192,7 @@
         <v>1.0000495000495E-2</v>
       </c>
     </row>
-    <row r="362" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="362" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B362" t="s">
         <v>21</v>
       </c>
@@ -14044,6 +14208,9 @@
       <c r="I362" t="s">
         <v>225</v>
       </c>
+      <c r="J362">
+        <v>4.950004950005E-3</v>
+      </c>
       <c r="O362">
         <v>4.950004950005E-3</v>
       </c>
@@ -14060,7 +14227,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="363" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="363" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B363" t="s">
         <v>21</v>
       </c>
@@ -14076,6 +14243,9 @@
       <c r="I363" t="s">
         <v>225</v>
       </c>
+      <c r="J363">
+        <v>4.950004950005E-3</v>
+      </c>
       <c r="O363">
         <v>4.950004950005E-3</v>
       </c>
@@ -14092,7 +14262,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="364" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="364" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B364" t="s">
         <v>21</v>
       </c>
@@ -14108,6 +14278,9 @@
       <c r="I364" t="s">
         <v>225</v>
       </c>
+      <c r="J364">
+        <v>4.950004950005E-3</v>
+      </c>
       <c r="O364">
         <v>4.950004950005E-3</v>
       </c>
@@ -14124,7 +14297,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="365" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="365" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B365" t="s">
         <v>21</v>
       </c>
@@ -14140,6 +14313,9 @@
       <c r="I365" t="s">
         <v>229</v>
       </c>
+      <c r="J365">
+        <v>4.950004950005E-3</v>
+      </c>
       <c r="O365">
         <v>4.950004950005E-3</v>
       </c>
@@ -14156,7 +14332,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="366" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="366" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B366" t="s">
         <v>21</v>
       </c>
@@ -14172,6 +14348,9 @@
       <c r="I366" t="s">
         <v>229</v>
       </c>
+      <c r="J366">
+        <v>4.950004950005E-3</v>
+      </c>
       <c r="O366">
         <v>4.950004950005E-3</v>
       </c>
@@ -14188,7 +14367,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="367" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="367" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B367" t="s">
         <v>21</v>
       </c>
@@ -14204,6 +14383,9 @@
       <c r="I367" t="s">
         <v>229</v>
       </c>
+      <c r="J367">
+        <v>4.950004950005E-3</v>
+      </c>
       <c r="O367">
         <v>4.950004950005E-3</v>
       </c>
@@ -14220,7 +14402,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="368" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="368" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B368" t="s">
         <v>21</v>
       </c>
@@ -14236,6 +14418,9 @@
       <c r="I368" t="s">
         <v>233</v>
       </c>
+      <c r="J368">
+        <v>4.950004950005E-3</v>
+      </c>
       <c r="P368">
         <v>4.950004950005E-3</v>
       </c>
@@ -14252,7 +14437,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="369" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="369" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B369" t="s">
         <v>21</v>
       </c>
@@ -14268,6 +14453,9 @@
       <c r="I369" t="s">
         <v>233</v>
       </c>
+      <c r="J369">
+        <v>4.950004950005E-3</v>
+      </c>
       <c r="P369">
         <v>4.950004950005E-3</v>
       </c>
@@ -14284,7 +14472,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="370" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="370" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B370" t="s">
         <v>21</v>
       </c>
@@ -14300,6 +14488,9 @@
       <c r="I370" t="s">
         <v>233</v>
       </c>
+      <c r="J370">
+        <v>4.950004950005E-3</v>
+      </c>
       <c r="P370">
         <v>4.950004950005E-3</v>
       </c>
@@ -14316,7 +14507,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="371" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="371" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B371" t="s">
         <v>21</v>
       </c>
@@ -14332,6 +14523,9 @@
       <c r="I371" t="s">
         <v>237</v>
       </c>
+      <c r="J371">
+        <v>4.950004950005E-4</v>
+      </c>
       <c r="N371">
         <v>6.435006435006E-4</v>
       </c>
@@ -14348,7 +14542,7 @@
         <v>9.9998267498267492E-3</v>
       </c>
     </row>
-    <row r="372" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="372" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B372" t="s">
         <v>21</v>
       </c>
@@ -14364,6 +14558,9 @@
       <c r="I372" t="s">
         <v>237</v>
       </c>
+      <c r="J372">
+        <v>4.950004950005E-4</v>
+      </c>
       <c r="N372">
         <v>6.435006435006E-4</v>
       </c>
@@ -14380,7 +14577,7 @@
         <v>9.9998267498267492E-3</v>
       </c>
     </row>
-    <row r="373" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="373" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B373" t="s">
         <v>21</v>
       </c>
@@ -14396,6 +14593,9 @@
       <c r="I373" t="s">
         <v>237</v>
       </c>
+      <c r="J373">
+        <v>4.950004950005E-4</v>
+      </c>
       <c r="N373">
         <v>6.435006435006E-4</v>
       </c>
@@ -14412,7 +14612,7 @@
         <v>9.9998267498267492E-3</v>
       </c>
     </row>
-    <row r="374" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="374" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B374" t="s">
         <v>21</v>
       </c>
@@ -14428,6 +14628,9 @@
       <c r="I374" t="s">
         <v>241</v>
       </c>
+      <c r="J374">
+        <v>4.950004950005E-4</v>
+      </c>
       <c r="S374">
         <v>4.950004950005E-3</v>
       </c>
@@ -14444,7 +14647,7 @@
         <v>1.0000495000495E-2</v>
       </c>
     </row>
-    <row r="375" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="375" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B375" t="s">
         <v>21</v>
       </c>
@@ -14460,6 +14663,9 @@
       <c r="I375" t="s">
         <v>241</v>
       </c>
+      <c r="J375">
+        <v>4.950004950005E-4</v>
+      </c>
       <c r="S375">
         <v>4.950004950005E-3</v>
       </c>
@@ -14476,7 +14682,7 @@
         <v>1.0000495000495E-2</v>
       </c>
     </row>
-    <row r="376" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="376" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B376" t="s">
         <v>21</v>
       </c>
@@ -14492,6 +14698,9 @@
       <c r="I376" t="s">
         <v>241</v>
       </c>
+      <c r="J376">
+        <v>4.950004950005E-4</v>
+      </c>
       <c r="S376">
         <v>4.950004950005E-3</v>
       </c>
@@ -14524,6 +14733,9 @@
       <c r="I377" t="s">
         <v>245</v>
       </c>
+      <c r="J377">
+        <v>4.950004950005E-4</v>
+      </c>
       <c r="O377">
         <v>0.17325017325020001</v>
       </c>
@@ -14559,6 +14771,9 @@
       <c r="I378" t="s">
         <v>245</v>
       </c>
+      <c r="J378">
+        <v>4.950004950005E-4</v>
+      </c>
       <c r="O378">
         <v>0.17325017325020001</v>
       </c>
@@ -14594,6 +14809,9 @@
       <c r="I379" t="s">
         <v>245</v>
       </c>
+      <c r="J379">
+        <v>4.950004950005E-4</v>
+      </c>
       <c r="O379">
         <v>0.17325017325020001</v>
       </c>
@@ -14613,7 +14831,7 @@
         <v>9.9950499950499996E-3</v>
       </c>
     </row>
-    <row r="380" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="380" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B380" t="s">
         <v>21</v>
       </c>
@@ -14629,6 +14847,9 @@
       <c r="I380" t="s">
         <v>249</v>
       </c>
+      <c r="J380">
+        <v>4.950004950005E-3</v>
+      </c>
       <c r="K380">
         <v>4.950004950005E-3</v>
       </c>
@@ -14645,7 +14866,7 @@
         <v>9.9995049995050007E-3</v>
       </c>
     </row>
-    <row r="381" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="381" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B381" t="s">
         <v>21</v>
       </c>
@@ -14661,6 +14882,9 @@
       <c r="I381" t="s">
         <v>249</v>
       </c>
+      <c r="J381">
+        <v>4.950004950005E-3</v>
+      </c>
       <c r="K381">
         <v>4.950004950005E-3</v>
       </c>
@@ -14677,7 +14901,7 @@
         <v>9.9995049995050007E-3</v>
       </c>
     </row>
-    <row r="382" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="382" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B382" t="s">
         <v>21</v>
       </c>
@@ -14693,6 +14917,9 @@
       <c r="I382" t="s">
         <v>249</v>
       </c>
+      <c r="J382">
+        <v>4.950004950005E-3</v>
+      </c>
       <c r="K382">
         <v>4.950004950005E-3</v>
       </c>
@@ -14709,7 +14936,7 @@
         <v>9.9995049995050007E-3</v>
       </c>
     </row>
-    <row r="383" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="383" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B383" t="s">
         <v>21</v>
       </c>
@@ -14725,6 +14952,9 @@
       <c r="I383" t="s">
         <v>253</v>
       </c>
+      <c r="J383">
+        <v>4.950004950005E-4</v>
+      </c>
       <c r="K383">
         <v>4.950004950005E-4</v>
       </c>
@@ -14741,7 +14971,7 @@
         <v>9.9995049995050007E-3</v>
       </c>
     </row>
-    <row r="384" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="384" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B384" t="s">
         <v>21</v>
       </c>
@@ -14757,6 +14987,9 @@
       <c r="I384" t="s">
         <v>253</v>
       </c>
+      <c r="J384">
+        <v>4.950004950005E-4</v>
+      </c>
       <c r="K384">
         <v>4.950004950005E-4</v>
       </c>
@@ -14773,7 +15006,7 @@
         <v>9.9995049995050007E-3</v>
       </c>
     </row>
-    <row r="385" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="385" spans="2:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="B385" t="s">
         <v>21</v>
       </c>
@@ -14789,6 +15022,9 @@
       <c r="I385" t="s">
         <v>253</v>
       </c>
+      <c r="J385">
+        <v>4.950004950005E-4</v>
+      </c>
       <c r="K385">
         <v>4.950004950005E-4</v>
       </c>
@@ -14806,6 +15042,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:X385" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="8">
+      <filters>
+        <filter val="vi_bi_la"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>